<commit_message>
saveat ranges in scenario tables support
</commit_message>
<xml_diff>
--- a/cases/story_3/scenarios.xlsx
+++ b/cases/story_3/scenarios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\HetaSimulator.jl\cases\story_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\dev\HetaSimulator\cases\story_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BF4E0F6-A736-4076-B955-CBE9A7407758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -540,48 +539,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -896,17 +895,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -940,7 +939,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -957,7 +956,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -974,7 +973,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>

</xml_diff>